<commit_message>
Conditions in example-data with more meaningful/readible names
</commit_message>
<xml_diff>
--- a/exampleData/example.xlsx
+++ b/exampleData/example.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evakohnert/Documents/PhD/RPackages/CountSpores/exampleData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\clemens\Repositories\CountSpores\exampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73EF36A-BE6D-7E44-82CD-5DC89DD9B4E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F70B068F-0A12-9D49-A0C3-1A7BA9D2ACA8}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="33600" windowHeight="20538"/>
   </bookViews>
   <sheets>
     <sheet name="Exp_1" sheetId="1" r:id="rId1"/>
     <sheet name="Exp_2" sheetId="2" r:id="rId2"/>
     <sheet name="Exp_3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="28">
   <si>
     <t>A</t>
   </si>
@@ -105,11 +104,26 @@
   <si>
     <t>Seg_3_total</t>
   </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>KO_1</t>
+  </si>
+  <si>
+    <t>Another_KO</t>
+  </si>
+  <si>
+    <t>Overexpression</t>
+  </si>
+  <si>
+    <t>AnotherPertubation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -166,7 +180,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -477,16 +491,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982EBAE9-EA44-7A4B-B9FA-689F664A0BEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:A106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -515,9 +529,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -544,9 +558,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -573,9 +587,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -602,9 +616,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -631,9 +645,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -660,9 +674,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -689,9 +703,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -718,9 +732,9 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -747,9 +761,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -776,9 +790,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -805,9 +819,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -834,9 +848,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -863,9 +877,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -892,9 +906,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -921,9 +935,9 @@
         <v>578</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -950,9 +964,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -979,9 +993,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -1008,9 +1022,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -1037,9 +1051,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -1066,9 +1080,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -1095,9 +1109,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -1124,9 +1138,9 @@
         <v>636</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1153,9 +1167,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1182,9 +1196,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
@@ -1211,9 +1225,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
@@ -1240,9 +1254,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
@@ -1269,9 +1283,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -1298,9 +1312,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -1327,9 +1341,9 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1356,9 +1370,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -1385,9 +1399,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -1414,9 +1428,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1443,9 +1457,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -1472,9 +1486,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -1501,9 +1515,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -1530,9 +1544,9 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
@@ -1559,9 +1573,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -1588,9 +1602,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -1617,9 +1631,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1646,9 +1660,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
@@ -1675,9 +1689,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
@@ -1704,9 +1718,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -1733,9 +1747,9 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
@@ -1762,9 +1776,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -1791,9 +1805,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
@@ -1820,9 +1834,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
@@ -1849,9 +1863,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
         <v>0</v>
@@ -1878,9 +1892,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
@@ -1907,9 +1921,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
         <v>0</v>
@@ -1936,9 +1950,9 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -1965,9 +1979,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -1994,9 +2008,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -2023,9 +2037,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -2052,9 +2066,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -2081,9 +2095,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -2110,9 +2124,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -2139,9 +2153,9 @@
         <v>721</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -2168,9 +2182,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -2197,9 +2211,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -2226,9 +2240,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -2255,9 +2269,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -2284,9 +2298,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -2313,9 +2327,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -2342,9 +2356,9 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
         <v>0</v>
@@ -2371,9 +2385,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
@@ -2400,9 +2414,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B67" t="s">
         <v>0</v>
@@ -2429,9 +2443,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
         <v>0</v>
@@ -2458,9 +2472,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
@@ -2487,9 +2501,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
         <v>0</v>
@@ -2516,9 +2530,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B71" t="s">
         <v>0</v>
@@ -2545,9 +2559,9 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -2574,9 +2588,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -2603,9 +2617,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -2632,9 +2646,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -2661,9 +2675,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -2690,9 +2704,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -2719,9 +2733,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -2748,9 +2762,9 @@
         <v>3316</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2777,9 +2791,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A80" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2806,9 +2820,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2835,9 +2849,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -2864,9 +2878,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
@@ -2893,9 +2907,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -2922,9 +2936,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -2951,9 +2965,9 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B86" t="s">
         <v>0</v>
@@ -2980,9 +2994,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A87" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B87" t="s">
         <v>0</v>
@@ -3009,9 +3023,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A88" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B88" t="s">
         <v>0</v>
@@ -3038,9 +3052,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A89" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B89" t="s">
         <v>0</v>
@@ -3067,9 +3081,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B90" t="s">
         <v>0</v>
@@ -3096,9 +3110,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A91" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B91" t="s">
         <v>0</v>
@@ -3125,9 +3139,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A92" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B92" t="s">
         <v>0</v>
@@ -3154,9 +3168,9 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
@@ -3183,9 +3197,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A94" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
@@ -3212,9 +3226,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A95" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
@@ -3241,9 +3255,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A96" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -3270,9 +3284,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
@@ -3299,9 +3313,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
@@ -3328,9 +3342,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A99" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -3357,9 +3371,9 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A100" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B100" t="s">
         <v>7</v>
@@ -3386,9 +3400,9 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A101" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
@@ -3415,9 +3429,9 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A102" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -3444,9 +3458,9 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A103" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
@@ -3473,9 +3487,9 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A104" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -3502,9 +3516,9 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A105" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -3531,9 +3545,9 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A106" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
@@ -3567,16 +3581,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BFC276-EFDF-3647-A132-E4DA5E375883}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3605,7 +3619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3634,7 +3648,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3663,7 +3677,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3692,7 +3706,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3721,7 +3735,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3750,7 +3764,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3779,7 +3793,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3808,7 +3822,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3837,7 +3851,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3866,7 +3880,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3895,7 +3909,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3924,7 +3938,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3953,7 +3967,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3982,7 +3996,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -4011,7 +4025,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -4040,7 +4054,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -4069,7 +4083,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -4098,7 +4112,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4127,7 +4141,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4156,7 +4170,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4185,7 +4199,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4214,7 +4228,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -4243,7 +4257,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -4272,7 +4286,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -4301,7 +4315,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -4330,7 +4344,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -4359,7 +4373,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -4388,7 +4402,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -4417,7 +4431,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -4446,7 +4460,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -4475,7 +4489,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -4504,7 +4518,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -4533,7 +4547,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -4562,7 +4576,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -4591,7 +4605,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -4620,7 +4634,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -4649,7 +4663,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -4678,7 +4692,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -4707,7 +4721,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -4736,7 +4750,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -4765,7 +4779,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -4794,7 +4808,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -4823,7 +4837,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -4852,7 +4866,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -4881,7 +4895,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -4910,7 +4924,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -4968,7 +4982,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -4997,7 +5011,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -5026,7 +5040,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -5055,7 +5069,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -5084,7 +5098,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -5113,7 +5127,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -5142,7 +5156,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -5171,7 +5185,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -5200,7 +5214,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -5229,7 +5243,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -5258,7 +5272,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -5287,7 +5301,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -5316,7 +5330,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -5345,7 +5359,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -5374,7 +5388,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -5403,7 +5417,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -5432,7 +5446,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -5461,7 +5475,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -5490,7 +5504,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -5519,7 +5533,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -5548,7 +5562,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -5577,7 +5591,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -5606,7 +5620,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -5635,7 +5649,7 @@
         <v>4697</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -5664,7 +5678,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -5693,7 +5707,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -5722,7 +5736,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -5751,7 +5765,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -5780,7 +5794,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -5809,7 +5823,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -5838,7 +5852,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -5867,7 +5881,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -5896,7 +5910,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -5925,7 +5939,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -5954,7 +5968,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -5983,7 +5997,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -6012,7 +6026,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -6041,7 +6055,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -6070,7 +6084,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -6099,7 +6113,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -6128,7 +6142,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -6157,7 +6171,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -6186,7 +6200,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -6215,7 +6229,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -6244,7 +6258,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -6273,7 +6287,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -6302,7 +6316,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -6331,7 +6345,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -6360,7 +6374,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -6389,7 +6403,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -6418,7 +6432,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -6447,7 +6461,7 @@
         <v>3359</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -6476,7 +6490,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -6505,7 +6519,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -6534,7 +6548,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -6563,7 +6577,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -6592,7 +6606,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -6621,7 +6635,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -6656,16 +6670,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56968DCA-2019-3445-A481-8B5322E3D1BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6694,7 +6708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6723,7 +6737,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -6752,7 +6766,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -6781,7 +6795,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6810,7 +6824,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -6839,7 +6853,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -6868,7 +6882,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -6897,7 +6911,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -6926,7 +6940,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -6955,7 +6969,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -6984,7 +6998,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -7013,7 +7027,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -7042,7 +7056,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -7071,7 +7085,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -7100,7 +7114,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -7129,7 +7143,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -7158,7 +7172,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -7187,7 +7201,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -7216,7 +7230,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -7245,7 +7259,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -7274,7 +7288,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -7303,7 +7317,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -7332,7 +7346,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -7361,7 +7375,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -7390,7 +7404,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -7419,7 +7433,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -7448,7 +7462,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -7477,7 +7491,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -7506,7 +7520,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -7535,7 +7549,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -7564,7 +7578,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -7593,7 +7607,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -7622,7 +7636,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -7651,7 +7665,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -7680,7 +7694,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -7709,7 +7723,7 @@
         <v>3315</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -7738,7 +7752,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -7767,7 +7781,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -7796,7 +7810,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -7825,7 +7839,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -7854,7 +7868,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -7883,7 +7897,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -7912,7 +7926,7 @@
         <v>2806</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -7941,7 +7955,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -7970,7 +7984,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -7999,7 +8013,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -8028,7 +8042,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -8057,7 +8071,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -8086,7 +8100,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -8115,7 +8129,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -8144,7 +8158,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -8173,7 +8187,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -8202,7 +8216,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -8231,7 +8245,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -8260,7 +8274,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -8289,7 +8303,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -8318,7 +8332,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -8347,7 +8361,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -8376,7 +8390,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -8405,7 +8419,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -8434,7 +8448,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -8463,7 +8477,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -8492,7 +8506,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -8521,7 +8535,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -8550,7 +8564,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -8579,7 +8593,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -8608,7 +8622,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -8637,7 +8651,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -8666,7 +8680,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -8695,7 +8709,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -8724,7 +8738,7 @@
         <v>4143</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -8753,7 +8767,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A73" t="s">
         <v>15</v>
       </c>
@@ -8782,7 +8796,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -8811,7 +8825,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A75" t="s">
         <v>15</v>
       </c>
@@ -8840,7 +8854,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A76" t="s">
         <v>15</v>
       </c>
@@ -8869,7 +8883,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -8898,7 +8912,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -8927,7 +8941,7 @@
         <v>3292</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -8956,7 +8970,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -8985,7 +8999,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A81" t="s">
         <v>15</v>
       </c>
@@ -9014,7 +9028,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A82" t="s">
         <v>15</v>
       </c>
@@ -9043,7 +9057,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -9072,7 +9086,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -9101,7 +9115,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -9130,7 +9144,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -9159,7 +9173,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -9188,7 +9202,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -9217,7 +9231,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -9246,7 +9260,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -9275,7 +9289,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -9304,7 +9318,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -9333,7 +9347,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -9362,7 +9376,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -9391,7 +9405,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -9420,7 +9434,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -9449,7 +9463,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -9478,7 +9492,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -9507,7 +9521,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -9536,7 +9550,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -9565,7 +9579,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -9594,7 +9608,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -9623,7 +9637,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -9652,7 +9666,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -9681,7 +9695,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -9710,7 +9724,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.6">
       <c r="A106" t="s">
         <v>16</v>
       </c>

</xml_diff>